<commit_message>
Tehnicki dug i dnevnik projekta
</commit_message>
<xml_diff>
--- a/SonarCloud/Dnevnik_projekta_Andjela_Todoric_IT22_2018.xlsx
+++ b/SonarCloud/Dnevnik_projekta_Andjela_Todoric_IT22_2018.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="83">
   <si>
     <t>Upravljanje razvojem informacionih sistema</t>
   </si>
@@ -400,6 +400,18 @@
   </si>
   <si>
     <t>Uncommented code</t>
+  </si>
+  <si>
+    <t>23.02.2022.</t>
+  </si>
+  <si>
+    <t>S1125</t>
+  </si>
+  <si>
+    <t>Boolean literals should not be redudant</t>
+  </si>
+  <si>
+    <t>Remove unnercessary true value</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1197,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1196,8 +1208,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,74 +2226,194 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="14"/>
+      <c r="A29" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="17">
+        <v>2</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="14"/>
+      <c r="A30" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" s="17">
+        <v>1</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="14"/>
+      <c r="A31" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" s="17">
+        <v>1</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I31" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="14"/>
+      <c r="A32" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="17">
+        <v>1</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K32" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="14"/>
+      <c r="A33" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G33" s="17">
+        <v>2</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L33" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>

</xml_diff>